<commit_message>
pequeñas modificaciones de esteticas (nada de codigo añadido o quitado)
</commit_message>
<xml_diff>
--- a/Resumen_Subenciones.xlsx
+++ b/Resumen_Subenciones.xlsx
@@ -38,13 +38,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -74,8 +74,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>

</xml_diff>

<commit_message>
Creando una función que selecciona rangos de celdas
</commit_message>
<xml_diff>
--- a/Resumen_Subenciones.xlsx
+++ b/Resumen_Subenciones.xlsx
@@ -29,18 +29,12 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -66,7 +60,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -75,7 +69,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -477,13 +470,13 @@
           <t>AMPA AGORA</t>
         </is>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>560</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>2421.67</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="I7" s="3" t="n">
         <v>269.07</v>
       </c>
     </row>
@@ -493,13 +486,13 @@
           <t>AMPA ALDEBARAN</t>
         </is>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="3" t="n">
         <v>980.05</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>3107.05</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="I8" s="3" t="n">
         <v>388.38</v>
       </c>
     </row>
@@ -509,13 +502,13 @@
           <t>AMPA ANTONIO MACHADO</t>
         </is>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="3" t="n">
         <v>921</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>2344.99</v>
       </c>
-      <c r="I9" s="4" t="n">
+      <c r="I9" s="3" t="n">
         <v>234.5</v>
       </c>
     </row>
@@ -525,13 +518,13 @@
           <t>AMPA BACHILLER ALONSO LOPEZ</t>
         </is>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="3" t="n">
         <v>928</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>3200</v>
       </c>
-      <c r="I10" s="4" t="n">
+      <c r="I10" s="3" t="n">
         <v>457.14</v>
       </c>
     </row>
@@ -541,13 +534,13 @@
           <t>AMPA CASTILLA</t>
         </is>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="3" t="n">
         <v>840</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>2604.44</v>
       </c>
-      <c r="I11" s="4" t="n">
+      <c r="I11" s="3" t="n">
         <v>260.44</v>
       </c>
     </row>
@@ -557,13 +550,13 @@
           <t>AMPA DAOIZ Y VELARDE</t>
         </is>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="3" t="n">
         <v>689</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>3152.74</v>
       </c>
-      <c r="I12" s="4" t="n">
+      <c r="I12" s="3" t="n">
         <v>394.09</v>
       </c>
     </row>
@@ -573,13 +566,13 @@
           <t>AMPA EL CUQUILLO</t>
         </is>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="3" t="n">
         <v>610</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>1507.83</v>
       </c>
-      <c r="I13" s="4" t="n">
+      <c r="I13" s="3" t="n">
         <v>376.96</v>
       </c>
     </row>
@@ -589,13 +582,13 @@
           <t>AMPA EMILIO CASADO</t>
         </is>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="3" t="n">
         <v>1000</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>3015.67</v>
       </c>
-      <c r="I14" s="4" t="n">
+      <c r="I14" s="3" t="n">
         <v>376.96</v>
       </c>
     </row>
@@ -605,13 +598,13 @@
           <t>AMPA FAPA</t>
         </is>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="3" t="n">
         <v>1515</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>3198.43</v>
       </c>
-      <c r="I15" s="4" t="n">
+      <c r="I15" s="3" t="n">
         <v>1066.14</v>
       </c>
     </row>
@@ -621,13 +614,13 @@
           <t>AMPA FEDERICO GARCIA LORCA</t>
         </is>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="3" t="n">
         <v>1400</v>
       </c>
       <c r="H16" s="3" t="n">
         <v>1919.06</v>
       </c>
-      <c r="I16" s="4" t="n">
+      <c r="I16" s="3" t="n">
         <v>639.6900000000001</v>
       </c>
     </row>
@@ -637,13 +630,13 @@
           <t>AMPA GABRIEL Y GALAN</t>
         </is>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="3" t="n">
         <v>1151.51</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>2741.51</v>
       </c>
-      <c r="I17" s="4" t="n">
+      <c r="I17" s="3" t="n">
         <v>342.69</v>
       </c>
     </row>
@@ -653,13 +646,13 @@
           <t>AMPA GINER DE LOS RIOS</t>
         </is>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="3" t="n">
         <v>673</v>
       </c>
       <c r="H18" s="3" t="n">
         <v>2058</v>
       </c>
-      <c r="I18" s="4" t="n">
+      <c r="I18" s="3" t="n">
         <v>294</v>
       </c>
     </row>
@@ -669,13 +662,13 @@
           <t>AMPA JUAN XXIII</t>
         </is>
       </c>
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="3" t="n">
         <v>800</v>
       </c>
       <c r="H19" s="3" t="n">
         <v>1781.98</v>
       </c>
-      <c r="I19" s="4" t="n">
+      <c r="I19" s="3" t="n">
         <v>593.99</v>
       </c>
     </row>
@@ -685,13 +678,13 @@
           <t>AMPA LA CHOPERA</t>
         </is>
       </c>
-      <c r="G20" s="4" t="n">
+      <c r="G20" s="3" t="n">
         <v>990</v>
       </c>
       <c r="H20" s="3" t="n">
         <v>1430</v>
       </c>
-      <c r="I20" s="4" t="n">
+      <c r="I20" s="3" t="n">
         <v>476.67</v>
       </c>
     </row>
@@ -701,13 +694,13 @@
           <t>AMPA LUIS BUÑUEL</t>
         </is>
       </c>
-      <c r="G21" s="4" t="n">
+      <c r="G21" s="3" t="n">
         <v>625</v>
       </c>
       <c r="H21" s="3" t="n">
         <v>2081</v>
       </c>
-      <c r="I21" s="4" t="n">
+      <c r="I21" s="3" t="n">
         <v>208.1</v>
       </c>
     </row>
@@ -717,13 +710,13 @@
           <t>AMPA MIGUEL HERNANDEZ</t>
         </is>
       </c>
-      <c r="G22" s="4" t="n">
+      <c r="G22" s="3" t="n">
         <v>530</v>
       </c>
       <c r="H22" s="3" t="n">
         <v>2923.35</v>
       </c>
-      <c r="I22" s="4" t="n">
+      <c r="I22" s="3" t="n">
         <v>243.61</v>
       </c>
     </row>
@@ -733,13 +726,13 @@
           <t>AMPA MIRAFLORES</t>
         </is>
       </c>
-      <c r="G23" s="4" t="n">
+      <c r="G23" s="3" t="n">
         <v>1500</v>
       </c>
       <c r="H23" s="3" t="n">
         <v>2787.21</v>
       </c>
-      <c r="I23" s="4" t="n">
+      <c r="I23" s="3" t="n">
         <v>696.8</v>
       </c>
     </row>
@@ -749,13 +742,13 @@
           <t>AMPA PADRE  MANYANET</t>
         </is>
       </c>
-      <c r="G24" s="4" t="n">
+      <c r="G24" s="3" t="n">
         <v>803.8200000000001</v>
       </c>
       <c r="H24" s="3" t="n">
         <v>2695.82</v>
       </c>
-      <c r="I24" s="4" t="n">
+      <c r="I24" s="3" t="n">
         <v>673.96</v>
       </c>
     </row>
@@ -765,13 +758,13 @@
           <t>AMPA PARQUE CATALUÑA</t>
         </is>
       </c>
-      <c r="G25" s="4" t="n">
+      <c r="G25" s="3" t="n">
         <v>995</v>
       </c>
       <c r="H25" s="3" t="n">
         <v>2604.44</v>
       </c>
-      <c r="I25" s="4" t="n">
+      <c r="I25" s="3" t="n">
         <v>325.56</v>
       </c>
     </row>
@@ -781,13 +774,13 @@
           <t>AMPA PROFESOR TIERNO GALVÁN</t>
         </is>
       </c>
-      <c r="G26" s="4" t="n">
+      <c r="G26" s="3" t="n">
         <v>306</v>
       </c>
       <c r="H26" s="3" t="n">
         <v>1286</v>
       </c>
-      <c r="I26" s="4" t="n">
+      <c r="I26" s="3" t="n">
         <v>214.33</v>
       </c>
     </row>
@@ -797,13 +790,13 @@
           <t>AMPA RIVENDEL</t>
         </is>
       </c>
-      <c r="G27" s="4" t="n">
+      <c r="G27" s="3" t="n">
         <v>794</v>
       </c>
       <c r="H27" s="3" t="n">
         <v>2200</v>
       </c>
-      <c r="I27" s="4" t="n">
+      <c r="I27" s="3" t="n">
         <v>275</v>
       </c>
     </row>
@@ -813,13 +806,13 @@
           <t>AMPA SAN ANTONIO</t>
         </is>
       </c>
-      <c r="G28" s="4" t="n">
+      <c r="G28" s="3" t="n">
         <v>895</v>
       </c>
       <c r="H28" s="3" t="n">
         <v>2101.83</v>
       </c>
-      <c r="I28" s="4" t="n">
+      <c r="I28" s="3" t="n">
         <v>700.61</v>
       </c>
     </row>
@@ -829,13 +822,13 @@
           <t>AMPA SEIS DE DICIEMBRE</t>
         </is>
       </c>
-      <c r="G29" s="4" t="n">
+      <c r="G29" s="3" t="n">
         <v>518</v>
       </c>
       <c r="H29" s="3" t="n">
         <v>1950</v>
       </c>
-      <c r="I29" s="4" t="n">
+      <c r="I29" s="3" t="n">
         <v>325</v>
       </c>
     </row>
@@ -845,13 +838,13 @@
           <t>AMPA SEVERO OCHOA</t>
         </is>
       </c>
-      <c r="G30" s="4" t="n">
+      <c r="G30" s="3" t="n">
         <v>981.97</v>
       </c>
       <c r="H30" s="3" t="n">
         <v>3563.97</v>
       </c>
-      <c r="I30" s="4" t="n">
+      <c r="I30" s="3" t="n">
         <v>356.4</v>
       </c>
     </row>
@@ -861,13 +854,13 @@
           <t>AMPA VALDELAPARRA</t>
         </is>
       </c>
-      <c r="G31" s="4" t="n">
+      <c r="G31" s="3" t="n">
         <v>685</v>
       </c>
       <c r="H31" s="3" t="n">
         <v>2465</v>
       </c>
-      <c r="I31" s="4" t="n">
+      <c r="I31" s="3" t="n">
         <v>352.14</v>
       </c>
     </row>
@@ -877,13 +870,13 @@
           <t>AMPA VALDEPALITOS</t>
         </is>
       </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="3" t="n">
         <v>690</v>
       </c>
       <c r="H32" s="3" t="n">
         <v>3929.5</v>
       </c>
-      <c r="I32" s="4" t="n">
+      <c r="I32" s="3" t="n">
         <v>231.15</v>
       </c>
     </row>
@@ -893,13 +886,13 @@
           <t>AMPA VIRGEN DE LA PAZ</t>
         </is>
       </c>
-      <c r="G33" s="4" t="n">
+      <c r="G33" s="3" t="n">
         <v>927.45</v>
       </c>
       <c r="H33" s="3" t="n">
         <v>1416.45</v>
       </c>
-      <c r="I33" s="4" t="n">
+      <c r="I33" s="3" t="n">
         <v>283.29</v>
       </c>
     </row>

</xml_diff>